<commit_message>
Refactor R analysis for OXXO cohort intensity plots
Rewrote and expanded the R script to generate cohort-based OXXO intensity plots using summarized panel data, improved color and shape mapping for cohorts, and added code to save the resulting plot. Also updated oxxo_counts.csv to correct several data entries for 2011, ensuring consistency with the new analysis.
</commit_message>
<xml_diff>
--- a/data/controles_results/difmedias_controles_baselines_fixed_2011.xlsx
+++ b/data/controles_results/difmedias_controles_baselines_fixed_2011.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="224" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="252" uniqueCount="112">
   <si>
     <t/>
   </si>
@@ -63,7 +63,13 @@
     <t>accesibilidad_arterial_dummy</t>
   </si>
   <si>
-    <t xml:space="preserve">If the table includes missing values (.n, .o, .v etc.) see the Missing values section in the help file for the Stata command iebaltab for definitions of these values. Significance: ***=.01, **=.05, *=.1. Full user input as written by user: [iebaltab poblacion_urbana_2009 poblacion_por_localidad_2005 poblacion_2005 personas_por_localidad_2007 personas_por_hogar_2007_localida num_est_transmi icv_2007_localidad gasto_promedio_mensual_2007_loca estrato_mean densidad_urbana_2009 area_urbana_2009 acceso_transmi accesibilidad_arterial accesibilidad_arterial_dummy , groupvar(dummy_oxxo) control(0) savexlsx(difmedias_controles_baselines_fixed_2011) replace] </t>
+    <t>total_personas</t>
+  </si>
+  <si>
+    <t>ingreso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the table includes missing values (.n, .o, .v etc.) see the Missing values section in the help file for the Stata command iebaltab for definitions of these values. Significance: ***=.01, **=.05, *=.1. Full user input as written by user: [iebaltab poblacion_urbana_2009 poblacion_por_localidad_2005 poblacion_2005 personas_por_localidad_2007 personas_por_hogar_2007_localida num_est_transmi icv_2007_localidad gasto_promedio_mensual_2007_loca estrato_mean densidad_urbana_2009 area_urbana_2009 acceso_transmi accesibilidad_arterial accesibilidad_arterial_dummy total_personas ingreso , groupvar(dummy_oxxo) control(0) savexlsx(difmedias_controles_baselines_fixed_2011) replace] </t>
   </si>
   <si>
     <t>N</t>
@@ -168,6 +174,18 @@
     <t>(0.009)</t>
   </si>
   <si>
+    <t>3.526</t>
+  </si>
+  <si>
+    <t>(0.059)</t>
+  </si>
+  <si>
+    <t>2.277</t>
+  </si>
+  <si>
+    <t>(0.044)</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
@@ -261,6 +279,15 @@
     <t>(0.000)</t>
   </si>
   <si>
+    <t>4.016</t>
+  </si>
+  <si>
+    <t>(0.097)</t>
+  </si>
+  <si>
+    <t>3.102</t>
+  </si>
+  <si>
     <t>896</t>
   </si>
   <si>
@@ -316,6 +343,12 @@
   </si>
   <si>
     <t>0.072</t>
+  </si>
+  <si>
+    <t>0.490</t>
+  </si>
+  <si>
+    <t>0.825**</t>
   </si>
 </sst>
 </file>
@@ -359,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -373,19 +406,19 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
@@ -396,19 +429,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
@@ -416,22 +449,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
@@ -439,22 +472,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
@@ -465,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -485,22 +518,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
@@ -511,13 +544,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -531,22 +564,22 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
@@ -557,13 +590,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -577,22 +610,22 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11">
@@ -603,13 +636,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -623,22 +656,22 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -649,13 +682,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -669,22 +702,22 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15">
@@ -695,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -715,22 +748,22 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17">
@@ -741,13 +774,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
@@ -761,22 +794,22 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19">
@@ -787,13 +820,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
         <v>0</v>
@@ -807,22 +840,22 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -833,13 +866,13 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
         <v>0</v>
@@ -853,22 +886,22 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23">
@@ -879,13 +912,13 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
         <v>0</v>
@@ -899,22 +932,22 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25">
@@ -925,13 +958,13 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
         <v>0</v>
@@ -945,22 +978,22 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G26" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27">
@@ -971,13 +1004,13 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F27" t="s">
         <v>0</v>
@@ -991,22 +1024,22 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G28" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29">
@@ -1017,13 +1050,13 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
         <v>0</v>
@@ -1037,22 +1070,22 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G30" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
@@ -1063,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
         <v>0</v>
@@ -1083,21 +1116,113 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="G32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>